<commit_message>
final report edits and started analysis R doc
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="2532"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8124" windowHeight="2532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="26">
   <si>
     <t>Run</t>
   </si>
@@ -43,34 +43,67 @@
     <t>Replicate 2 Results (Distance traveled, in)</t>
   </si>
   <si>
-    <t>45 degrees</t>
-  </si>
-  <si>
-    <t>Backward</t>
-  </si>
-  <si>
-    <t>9 inches</t>
-  </si>
-  <si>
     <t>35 grams</t>
   </si>
   <si>
-    <t>60 degrees</t>
-  </si>
-  <si>
-    <t>3 inches</t>
-  </si>
-  <si>
     <t>55 grams</t>
   </si>
   <si>
-    <t>Forward</t>
+    <t>0 inches</t>
+  </si>
+  <si>
+    <t>30 degrees</t>
+  </si>
+  <si>
+    <t>55 degrees</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">D = </t>
+  </si>
+  <si>
+    <t>Change in angle</t>
+  </si>
+  <si>
+    <t>Change in base height</t>
+  </si>
+  <si>
+    <t>Change in weight of the payload (pig)</t>
+  </si>
+  <si>
+    <t>Change in preload (pull back length)</t>
+  </si>
+  <si>
+    <t>18 inches</t>
+  </si>
+  <si>
+    <t>8 inches</t>
+  </si>
+  <si>
+    <t>6.5 inches</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,8 +444,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -777,6 +816,56 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -824,12 +913,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -839,10 +924,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
@@ -857,6 +938,34 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1211,368 +1320,550 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.33203125" customWidth="1"/>
-    <col min="7" max="7" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.33203125" customWidth="1"/>
+    <col min="13" max="14" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="H1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="I1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="J1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="K1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="7" t="s">
+      <c r="L1" s="13"/>
+      <c r="M1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="N1" s="33" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="15">
+        <f>5*12</f>
+        <v>60</v>
+      </c>
+      <c r="N2" s="15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="14"/>
+      <c r="M3" s="16">
+        <v>27</v>
+      </c>
+      <c r="N3" s="16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="L4" s="14"/>
+      <c r="M4" s="16">
         <v>9</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="N4" s="16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>4</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="I5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="16">
+        <f>7.5*12</f>
+        <v>90</v>
+      </c>
+      <c r="N5" s="16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="I6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="14"/>
+      <c r="M6" s="16">
+        <f>4.75*12</f>
+        <v>57</v>
+      </c>
+      <c r="N6" s="16">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2">
+        <v>6</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="16">
+        <f>5*12</f>
+        <v>60</v>
+      </c>
+      <c r="N7" s="16">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2">
+        <v>7</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="L8" s="14"/>
+      <c r="M8" s="16">
+        <f>2.75*12</f>
+        <v>33</v>
+      </c>
+      <c r="N8" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2">
+        <v>8</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="14"/>
+      <c r="M9" s="16">
+        <v>13</v>
+      </c>
+      <c r="N9" s="16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2">
+        <v>9</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="14"/>
+      <c r="M10" s="16">
+        <f>2.75*12</f>
+        <v>33</v>
+      </c>
+      <c r="N10" s="16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2">
+        <v>10</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="16">
+        <v>32</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G12" s="2">
+        <v>11</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="14"/>
+      <c r="M12" s="16">
+        <v>36</v>
+      </c>
+      <c r="N12" s="16">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G13" s="2">
         <v>12</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="H13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="I13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="14"/>
+      <c r="M13" s="16">
+        <f>4.5*12</f>
+        <v>54</v>
+      </c>
+      <c r="N13" s="16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G14" s="2">
+        <v>13</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="I14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="L14" s="14"/>
+      <c r="M14" s="16">
+        <f>1.8*12</f>
+        <v>21.6</v>
+      </c>
+      <c r="N14" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G15" s="2">
+        <v>14</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="K15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="14"/>
+      <c r="M15" s="16">
+        <f>2.25*12</f>
+        <v>27</v>
+      </c>
+      <c r="N15" s="16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G16" s="2">
+        <v>15</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="14"/>
+      <c r="M16" s="16">
+        <v>37</v>
+      </c>
+      <c r="N16" s="16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="3">
+        <v>16</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L17" s="14"/>
+      <c r="M17" s="17">
+        <v>47</v>
+      </c>
+      <c r="N17" s="17">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>6.5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>6.5</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="G20" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="H20" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="23"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G21" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="18"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="H21" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="19"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G22" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5">
+      <c r="H22" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="19"/>
+    </row>
+    <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
+      <c r="H23" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="H23:K23"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
done working on the r files and excel files for the morning
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="25">
   <si>
     <t>Run</t>
   </si>
@@ -94,17 +94,14 @@
     <t>6.5 inches</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Low</t>
+    <t>MISSING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,8 +236,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,8 +461,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5757"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -863,6 +886,68 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -913,7 +998,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -944,9 +1029,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
@@ -966,6 +1048,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1013,6 +1134,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5757"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1324,11 +1450,13 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="5.77734375" customWidth="1"/>
     <col min="7" max="7" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
@@ -1338,32 +1466,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G1" s="34" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="35" t="s">
+      <c r="B1" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="D1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="E1" s="33" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>4</v>
+      </c>
       <c r="L1" s="13"/>
-      <c r="M1" s="33" t="s">
+      <c r="M1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="N1" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" s="61">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24">
+        <f>IF(H2="30 degrees",-1,1)</f>
+        <v>-1</v>
+      </c>
+      <c r="C2" s="22">
+        <f>IF(I2="8 inches",-1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="22">
+        <f>IF(J2="0 inches",-1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="23">
+        <f>IF(K2="35 grams",-1,1)</f>
+        <v>-1</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -1390,8 +1549,24 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>2</v>
+      </c>
+      <c r="B3" s="25">
+        <f t="shared" ref="B3:B17" si="0">IF(H3="30 degrees",-1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="18">
+        <f t="shared" ref="C3:C17" si="1">IF(I3="8 inches",-1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="18">
+        <f t="shared" ref="D3:D17" si="2">IF(J3="0 inches",-1,1)</f>
+        <v>-1</v>
+      </c>
+      <c r="E3" s="19">
+        <f t="shared" ref="E3:E17" si="3">IF(K3="35 grams",-1,1)</f>
+        <v>-1</v>
       </c>
       <c r="G3" s="2">
         <v>2</v>
@@ -1417,8 +1592,24 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>3</v>
+      </c>
+      <c r="B4" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C4" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D4" s="18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="19">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G4" s="2">
         <v>3</v>
@@ -1444,8 +1635,24 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>4</v>
+      </c>
+      <c r="B5" s="25">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C5" s="18">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D5" s="18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="19">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G5" s="2">
         <v>4</v>
@@ -1472,8 +1679,24 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="2">
         <v>5</v>
+      </c>
+      <c r="B6" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C6" s="18">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D6" s="18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="19">
+        <f t="shared" si="3"/>
+        <v>-1</v>
       </c>
       <c r="G6" s="2">
         <v>5</v>
@@ -1500,8 +1723,24 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>6</v>
+      </c>
+      <c r="B7" s="25">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C7" s="18">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D7" s="18">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E7" s="19">
+        <f t="shared" si="3"/>
+        <v>-1</v>
       </c>
       <c r="G7" s="2">
         <v>6</v>
@@ -1528,8 +1767,24 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>7</v>
+      </c>
+      <c r="B8" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C8" s="18">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D8" s="18">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E8" s="19">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G8" s="2">
         <v>7</v>
@@ -1556,8 +1811,24 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>8</v>
+      </c>
+      <c r="B9" s="25">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C9" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D9" s="18">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E9" s="19">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G9" s="2">
         <v>8</v>
@@ -1583,8 +1854,24 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>9</v>
+      </c>
+      <c r="B10" s="25">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C10" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="18">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E10" s="19">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G10" s="2">
         <v>9</v>
@@ -1611,8 +1898,24 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>10</v>
+      </c>
+      <c r="B11" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C11" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D11" s="18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="19">
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G11" s="2">
         <v>10</v>
@@ -1638,6 +1941,28 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="60">
+        <v>11</v>
+      </c>
+      <c r="B12" s="59">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C12" s="58">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="58">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="47">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="57">
+        <v>-1</v>
+      </c>
       <c r="G12" s="2">
         <v>11</v>
       </c>
@@ -1650,7 +1975,7 @@
       <c r="J12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="47" t="s">
         <v>8</v>
       </c>
       <c r="L12" s="14"/>
@@ -1662,6 +1987,25 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="25">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C13" s="18">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D13" s="18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="19">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="G13" s="2">
         <v>12</v>
       </c>
@@ -1687,6 +2031,25 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C14" s="18">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D14" s="18">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E14" s="19">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="G14" s="2">
         <v>13</v>
       </c>
@@ -1712,6 +2075,25 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C15" s="18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="18">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E15" s="19">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
       <c r="G15" s="2">
         <v>14</v>
       </c>
@@ -1737,6 +2119,28 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="60">
+        <v>15</v>
+      </c>
+      <c r="B16" s="59">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="C16" s="58">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D16" s="58">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E16" s="47">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="57">
+        <v>-1</v>
+      </c>
       <c r="G16" s="2">
         <v>15</v>
       </c>
@@ -1749,7 +2153,7 @@
       <c r="J16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" s="47" t="s">
         <v>8</v>
       </c>
       <c r="L16" s="14"/>
@@ -1761,6 +2165,25 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C17" s="20">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="D17" s="20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="21">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
       <c r="G17" s="3">
         <v>16</v>
       </c>
@@ -1770,7 +2193,7 @@
       <c r="I17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="37" t="s">
+      <c r="J17" s="34" t="s">
         <v>21</v>
       </c>
       <c r="K17" s="12" t="s">
@@ -1786,75 +2209,87 @@
     </row>
     <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>6.5</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="B19" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C19">
-        <v>6.5</v>
-      </c>
-      <c r="G19" s="24" t="s">
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="50"/>
+      <c r="G19" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="26"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="37"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="G20" s="30" t="s">
+      <c r="B20" s="51">
+        <v>-1</v>
+      </c>
+      <c r="C20" s="52">
+        <v>-1</v>
+      </c>
+      <c r="D20" s="52">
+        <v>-1</v>
+      </c>
+      <c r="E20" s="53">
+        <v>-1</v>
+      </c>
+      <c r="G20" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="23"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="40"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G21" s="31" t="s">
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="54">
+        <v>-1</v>
+      </c>
+      <c r="C21" s="55">
+        <v>1</v>
+      </c>
+      <c r="D21" s="55">
+        <v>1</v>
+      </c>
+      <c r="E21" s="56">
+        <v>-1</v>
+      </c>
+      <c r="G21" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="28" t="s">
+      <c r="H21" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="43"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="28" t="s">
+      <c r="H22" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="43"/>
     </row>
     <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G23" s="32" t="s">
+      <c r="G23" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="21"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1865,5 +2300,6 @@
     <mergeCell ref="H23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to all docs
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="24">
   <si>
     <t>Run</t>
   </si>
@@ -92,16 +92,13 @@
   </si>
   <si>
     <t>6.5 inches</t>
-  </si>
-  <si>
-    <t>MISSING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,16 +239,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="40">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,20 +450,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF5757"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="38">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -883,55 +860,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -998,7 +926,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1049,31 +977,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="35" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1088,6 +998,15 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1450,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1467,10 +1386,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="32" t="s">
@@ -1506,7 +1425,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="50">
+      <c r="A2" s="36">
         <v>1</v>
       </c>
       <c r="B2" s="24">
@@ -1942,25 +1861,25 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="49">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="48">
+      <c r="B12" s="52">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="C12" s="47">
+      <c r="C12" s="53">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="53">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E12" s="36">
-        <v>-1</v>
-      </c>
-      <c r="F12" s="46"/>
+      <c r="E12" s="54">
+        <v>-1</v>
+      </c>
+      <c r="F12" s="51"/>
       <c r="G12" s="2">
         <v>11</v>
       </c>
@@ -2117,25 +2036,25 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="49">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="52">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="53">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="53">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
-      <c r="E16" s="36">
-        <v>-1</v>
-      </c>
-      <c r="F16" s="46"/>
+      <c r="E16" s="54">
+        <v>-1</v>
+      </c>
+      <c r="F16" s="51"/>
       <c r="G16" s="2">
         <v>15</v>
       </c>
@@ -2204,87 +2123,69 @@
     </row>
     <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-      <c r="G19" s="53" t="s">
+      <c r="B19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="G19" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="55"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="41"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="40">
-        <v>-1</v>
-      </c>
-      <c r="C20" s="41">
-        <v>-1</v>
-      </c>
-      <c r="D20" s="41">
-        <v>-1</v>
-      </c>
-      <c r="E20" s="42">
-        <v>-1</v>
-      </c>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
       <c r="G20" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="56" t="s">
+      <c r="H20" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="58"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="44"/>
     </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="43">
-        <v>-1</v>
-      </c>
-      <c r="C21" s="44">
-        <v>1</v>
-      </c>
-      <c r="D21" s="44">
-        <v>1</v>
-      </c>
-      <c r="E21" s="45">
-        <v>-1</v>
-      </c>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
       <c r="G21" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="59" t="s">
+      <c r="H21" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="61"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="47"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G22" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="59" t="s">
+      <c r="H22" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="60"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="61"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="47"/>
     </row>
     <row r="23" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G23" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="62" t="s">
+      <c r="H23" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="64"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>